<commit_message>
create contact and edit contact completed
</commit_message>
<xml_diff>
--- a/assets/downloadedFiles/xlList.xlsx
+++ b/assets/downloadedFiles/xlList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t/>
   </si>
@@ -38,34 +38,43 @@
     <t>PINCODE</t>
   </si>
   <si>
+    <t>VaishakT S</t>
+  </si>
+  <si>
+    <t>vaishak@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>2001-04-10</t>
+  </si>
+  <si>
+    <t>MarthandamTamil Nadu</t>
+  </si>
+  <si>
     <t>AnisreeS S</t>
   </si>
   <si>
     <t>anisree@gmail.com</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>2024-07-12</t>
-  </si>
-  <si>
-    <t>S S NilayamUdhimoodu</t>
-  </si>
-  <si>
-    <t>VaishakT S</t>
-  </si>
-  <si>
-    <t>vaishak@gmail.com</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>2001-04-10</t>
-  </si>
-  <si>
-    <t>MarthandamTamil Nadu</t>
+    <t>2000-07-12</t>
+  </si>
+  <si>
+    <t>VenjaranmooduTVM</t>
+  </si>
+  <si>
+    <t>ArjunK</t>
+  </si>
+  <si>
+    <t>arjun@gmail.com</t>
+  </si>
+  <si>
+    <t>2001-04-16</t>
+  </si>
+  <si>
+    <t>AnachalIdukki</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -156,7 +165,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>9.63852741E9</v>
+        <v>9.87654321E9</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -168,7 +177,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>123465.0</v>
+        <v>654321.0</v>
       </c>
     </row>
     <row r="3">
@@ -179,18 +188,41 @@
         <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>1.111111111E9</v>
+        <v>9.87654321E9</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="n">
+        <v>654321.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="n">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.63852741E9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="n">
         <v>123456.0</v>
       </c>
     </row>

</xml_diff>